<commit_message>
Atualizada a ATA 24-03-2021
</commit_message>
<xml_diff>
--- a/Sprint1/ATA's/20210323_Protocolo_Reunião_Agro_Cane.xlsx
+++ b/Sprint1/ATA's/20210323_Protocolo_Reunião_Agro_Cane.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Agro Cane (PI) - Sprint 2\Agro-Cane---Sprint-2\Sprint1\ATA's\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA4D8D2-1CAC-4F18-B375-C7FDC7A05039}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF47EF8-93D4-48AB-97DB-3C4628A8C468}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="840" windowWidth="18285" windowHeight="15360" xr2:uid="{4A4715A1-8DB2-4B72-B77A-B9437366CE44}"/>
+    <workbookView xWindow="38280" yWindow="660" windowWidth="20640" windowHeight="11160" xr2:uid="{4A4715A1-8DB2-4B72-B77A-B9437366CE44}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>ATA de Reunião de Projeto</t>
   </si>
@@ -85,6 +85,27 @@
   </si>
   <si>
     <t>Melhorar a experiência no desenvolvimento da colheita utilizando como metódo a análise de temperatura e umidade dos plantios.</t>
+  </si>
+  <si>
+    <t>Elaborar HLD individualmente para discussões</t>
+  </si>
+  <si>
+    <t>Todos</t>
+  </si>
+  <si>
+    <t>Reunir informações de cada colaborador e unificar em um arquivo (HLD)</t>
+  </si>
+  <si>
+    <t>Elaborar LLD individualmente para discussões</t>
+  </si>
+  <si>
+    <t>Reunir informações de cada colaborador e unificar em um arquivo (LDD)</t>
+  </si>
+  <si>
+    <t>Entregar HLD &amp; LLD (Tecnologia da Informação)</t>
+  </si>
+  <si>
+    <t>Grupo se reuniu para discutir e elaborar o HLD &amp; LLD da aula de Tecnologia da Informação, entretanto algumas questões surgiram e o tempo pré-determinado para a reunião foi excedido, portanto o grupo deciciu que todos fariam individualmente o HLD e na próxima reunião decidiriamos.</t>
   </si>
 </sst>
 </file>
@@ -375,7 +396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -402,6 +423,57 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -444,9 +516,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -462,53 +531,14 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1023,8 +1053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7B51128-EAF0-4626-A17F-BDF6B8FE3400}">
   <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="145" zoomScaleNormal="100" zoomScaleSheetLayoutView="145" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1048,95 +1078,95 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
       <c r="K2" s="6"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
       <c r="K3" s="6"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
       <c r="K4" s="6"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
       <c r="K5" s="6"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
       <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
       <c r="K7" s="6"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
       <c r="K8" s="6"/>
     </row>
     <row r="9" spans="1:11" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1154,61 +1184,61 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="29" t="s">
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="46"/>
       <c r="K10" s="6"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="31" t="s">
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="47"/>
+      <c r="J11" s="47"/>
       <c r="K11" s="6"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
+      <c r="J12" s="47"/>
       <c r="K12" s="6"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="30"/>
-      <c r="D13" s="40">
+      <c r="C13" s="16"/>
+      <c r="D13" s="18">
         <v>44278</v>
       </c>
-      <c r="E13" s="40"/>
+      <c r="E13" s="18"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
@@ -1218,70 +1248,70 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="46"/>
+      <c r="I14" s="46"/>
+      <c r="J14" s="46"/>
       <c r="K14" s="6"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
-      <c r="B15" s="50" t="s">
+      <c r="B15" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="51"/>
+      <c r="C15" s="32"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="34" t="s">
+      <c r="E15" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="34"/>
+      <c r="F15" s="50"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="34" t="s">
+      <c r="H15" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="I15" s="34"/>
+      <c r="I15" s="50"/>
       <c r="J15" s="2"/>
       <c r="K15" s="6"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="33"/>
+      <c r="C16" s="49"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="35" t="s">
+      <c r="E16" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="35"/>
+      <c r="F16" s="51"/>
       <c r="G16" s="3"/>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="I16" s="35"/>
+      <c r="I16" s="51"/>
       <c r="J16" s="4"/>
       <c r="K16" s="6"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
-      <c r="J17" s="49"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="30"/>
       <c r="K17" s="6"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1299,17 +1329,17 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="36"/>
       <c r="K19" s="6"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1328,117 +1358,119 @@
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="7"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="22"/>
+      <c r="C21" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="39"/>
       <c r="J21" s="7"/>
       <c r="K21" s="6"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="7"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="25"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="42"/>
       <c r="J22" s="7"/>
       <c r="K22" s="6"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="7"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
-      <c r="I23" s="25"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="41"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="41"/>
+      <c r="I23" s="42"/>
       <c r="J23" s="7"/>
       <c r="K23" s="6"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="7"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="25"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="41"/>
+      <c r="I24" s="42"/>
       <c r="J24" s="7"/>
       <c r="K24" s="6"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="7"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="25"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="41"/>
+      <c r="G25" s="41"/>
+      <c r="H25" s="41"/>
+      <c r="I25" s="42"/>
       <c r="J25" s="7"/>
       <c r="K25" s="6"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="7"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="25"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="41"/>
+      <c r="G26" s="41"/>
+      <c r="H26" s="41"/>
+      <c r="I26" s="42"/>
       <c r="J26" s="7"/>
       <c r="K26" s="6"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="7"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="25"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="41"/>
+      <c r="I27" s="42"/>
       <c r="J27" s="7"/>
       <c r="K27" s="6"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="7"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="25"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
+      <c r="G28" s="41"/>
+      <c r="H28" s="41"/>
+      <c r="I28" s="42"/>
       <c r="J28" s="7"/>
       <c r="K28" s="6"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="7"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="28"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="45"/>
       <c r="J29" s="7"/>
       <c r="K29" s="6"/>
     </row>
@@ -1457,241 +1489,271 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
-      <c r="B31" s="42" t="s">
+      <c r="B31" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="42"/>
-      <c r="D31" s="42"/>
-      <c r="E31" s="42"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="42"/>
-      <c r="H31" s="42"/>
-      <c r="I31" s="42"/>
-      <c r="J31" s="42"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
       <c r="K31" s="6"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
-      <c r="B32" s="43" t="s">
+      <c r="B32" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="43"/>
-      <c r="D32" s="43"/>
-      <c r="E32" s="43"/>
-      <c r="F32" s="43"/>
-      <c r="G32" s="44" t="s">
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="H32" s="44"/>
-      <c r="I32" s="45" t="s">
+      <c r="H32" s="23"/>
+      <c r="I32" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="J32" s="45"/>
+      <c r="J32" s="24"/>
       <c r="K32" s="6"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
-      <c r="B33" s="46"/>
-      <c r="C33" s="46"/>
-      <c r="D33" s="46"/>
-      <c r="E33" s="46"/>
-      <c r="F33" s="46"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="36"/>
-      <c r="I33" s="37"/>
-      <c r="J33" s="37"/>
+      <c r="B33" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="52"/>
+      <c r="D33" s="52"/>
+      <c r="E33" s="52"/>
+      <c r="F33" s="52"/>
+      <c r="G33" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="H33" s="53"/>
+      <c r="I33" s="54">
+        <v>44279</v>
+      </c>
+      <c r="J33" s="54"/>
       <c r="K33" s="6"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
-      <c r="B34" s="46"/>
-      <c r="C34" s="46"/>
-      <c r="D34" s="46"/>
-      <c r="E34" s="46"/>
-      <c r="F34" s="46"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="36"/>
-      <c r="I34" s="37"/>
-      <c r="J34" s="37"/>
+      <c r="B34" s="52"/>
+      <c r="C34" s="52"/>
+      <c r="D34" s="52"/>
+      <c r="E34" s="52"/>
+      <c r="F34" s="52"/>
+      <c r="G34" s="53"/>
+      <c r="H34" s="53"/>
+      <c r="I34" s="54"/>
+      <c r="J34" s="54"/>
       <c r="K34" s="6"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
-      <c r="B35" s="46"/>
-      <c r="C35" s="46"/>
-      <c r="D35" s="46"/>
-      <c r="E35" s="46"/>
-      <c r="F35" s="46"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="36"/>
-      <c r="I35" s="37"/>
-      <c r="J35" s="37"/>
+      <c r="B35" s="52"/>
+      <c r="C35" s="52"/>
+      <c r="D35" s="52"/>
+      <c r="E35" s="52"/>
+      <c r="F35" s="52"/>
+      <c r="G35" s="53"/>
+      <c r="H35" s="53"/>
+      <c r="I35" s="54"/>
+      <c r="J35" s="54"/>
       <c r="K35" s="6"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
-      <c r="B36" s="38"/>
-      <c r="C36" s="38"/>
-      <c r="D36" s="38"/>
-      <c r="E36" s="38"/>
-      <c r="F36" s="38"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="37"/>
-      <c r="J36" s="37"/>
+      <c r="B36" s="52" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" s="52"/>
+      <c r="D36" s="52"/>
+      <c r="E36" s="52"/>
+      <c r="F36" s="52"/>
+      <c r="G36" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="H36" s="53"/>
+      <c r="I36" s="54">
+        <v>44279</v>
+      </c>
+      <c r="J36" s="54"/>
       <c r="K36" s="6"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
-      <c r="B37" s="38"/>
-      <c r="C37" s="38"/>
-      <c r="D37" s="38"/>
-      <c r="E37" s="38"/>
-      <c r="F37" s="38"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="37"/>
-      <c r="J37" s="37"/>
+      <c r="B37" s="52"/>
+      <c r="C37" s="52"/>
+      <c r="D37" s="52"/>
+      <c r="E37" s="52"/>
+      <c r="F37" s="52"/>
+      <c r="G37" s="53"/>
+      <c r="H37" s="53"/>
+      <c r="I37" s="54"/>
+      <c r="J37" s="54"/>
       <c r="K37" s="6"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
-      <c r="B38" s="38"/>
-      <c r="C38" s="38"/>
-      <c r="D38" s="38"/>
-      <c r="E38" s="38"/>
-      <c r="F38" s="38"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="37"/>
-      <c r="J38" s="37"/>
+      <c r="B38" s="52"/>
+      <c r="C38" s="52"/>
+      <c r="D38" s="52"/>
+      <c r="E38" s="52"/>
+      <c r="F38" s="52"/>
+      <c r="G38" s="53"/>
+      <c r="H38" s="53"/>
+      <c r="I38" s="54"/>
+      <c r="J38" s="54"/>
       <c r="K38" s="6"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
-      <c r="B39" s="38"/>
-      <c r="C39" s="38"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="38"/>
-      <c r="F39" s="38"/>
-      <c r="G39" s="36"/>
-      <c r="H39" s="36"/>
-      <c r="I39" s="37"/>
-      <c r="J39" s="37"/>
+      <c r="B39" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="H39" s="26"/>
+      <c r="I39" s="27">
+        <v>44280</v>
+      </c>
+      <c r="J39" s="27"/>
       <c r="K39" s="6"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
-      <c r="B40" s="38"/>
-      <c r="C40" s="38"/>
-      <c r="D40" s="38"/>
-      <c r="E40" s="38"/>
-      <c r="F40" s="38"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="36"/>
-      <c r="I40" s="37"/>
-      <c r="J40" s="37"/>
+      <c r="B40" s="25"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="25"/>
+      <c r="F40" s="25"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="27"/>
+      <c r="J40" s="27"/>
       <c r="K40" s="6"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
-      <c r="B41" s="38"/>
-      <c r="C41" s="38"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="38"/>
-      <c r="F41" s="38"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="37"/>
-      <c r="J41" s="37"/>
+      <c r="B41" s="25"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="25"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="25"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="27"/>
+      <c r="J41" s="27"/>
       <c r="K41" s="6"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
-      <c r="B42" s="38"/>
-      <c r="C42" s="38"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="38"/>
-      <c r="F42" s="38"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="37"/>
-      <c r="J42" s="37"/>
+      <c r="B42" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C42" s="25"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="25"/>
+      <c r="F42" s="25"/>
+      <c r="G42" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="H42" s="26"/>
+      <c r="I42" s="27">
+        <v>44280</v>
+      </c>
+      <c r="J42" s="27"/>
       <c r="K42" s="6"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
-      <c r="B43" s="38"/>
-      <c r="C43" s="38"/>
-      <c r="D43" s="38"/>
-      <c r="E43" s="38"/>
-      <c r="F43" s="38"/>
-      <c r="G43" s="36"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="37"/>
-      <c r="J43" s="37"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="26"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="27"/>
       <c r="K43" s="6"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
-      <c r="B44" s="38"/>
-      <c r="C44" s="38"/>
-      <c r="D44" s="38"/>
-      <c r="E44" s="38"/>
-      <c r="F44" s="38"/>
-      <c r="G44" s="36"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="37"/>
-      <c r="J44" s="37"/>
+      <c r="B44" s="25"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="25"/>
+      <c r="E44" s="25"/>
+      <c r="F44" s="25"/>
+      <c r="G44" s="26"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
       <c r="K44" s="6"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
-      <c r="B45" s="38"/>
-      <c r="C45" s="38"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="38"/>
-      <c r="F45" s="38"/>
-      <c r="G45" s="36"/>
-      <c r="H45" s="36"/>
-      <c r="I45" s="37"/>
-      <c r="J45" s="37"/>
+      <c r="B45" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="26"/>
+      <c r="H45" s="26"/>
+      <c r="I45" s="27">
+        <v>44281</v>
+      </c>
+      <c r="J45" s="27"/>
       <c r="K45" s="6"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
-      <c r="B46" s="38"/>
-      <c r="C46" s="38"/>
-      <c r="D46" s="38"/>
-      <c r="E46" s="38"/>
-      <c r="F46" s="38"/>
-      <c r="G46" s="36"/>
-      <c r="H46" s="36"/>
-      <c r="I46" s="37"/>
-      <c r="J46" s="37"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="26"/>
+      <c r="H46" s="26"/>
+      <c r="I46" s="27"/>
+      <c r="J46" s="27"/>
       <c r="K46" s="6"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
-      <c r="B47" s="38"/>
-      <c r="C47" s="38"/>
-      <c r="D47" s="38"/>
-      <c r="E47" s="38"/>
-      <c r="F47" s="38"/>
-      <c r="G47" s="36"/>
-      <c r="H47" s="36"/>
-      <c r="I47" s="37"/>
-      <c r="J47" s="37"/>
+      <c r="B47" s="20"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="26"/>
+      <c r="H47" s="26"/>
+      <c r="I47" s="27"/>
+      <c r="J47" s="27"/>
       <c r="K47" s="6"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
-      <c r="B48" s="39" t="s">
+      <c r="B48" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C48" s="39"/>
-      <c r="D48" s="40"/>
-      <c r="E48" s="39"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="18">
+        <v>44279</v>
+      </c>
+      <c r="E48" s="17"/>
       <c r="F48" s="7"/>
       <c r="G48" s="7"/>
       <c r="H48" s="7"/>
@@ -1701,10 +1763,10 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
-      <c r="B49" s="30"/>
-      <c r="C49" s="30"/>
-      <c r="D49" s="30"/>
-      <c r="E49" s="30"/>
+      <c r="B49" s="16"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="16"/>
       <c r="F49" s="7"/>
       <c r="G49" s="7"/>
       <c r="H49" s="7"/>
@@ -1727,6 +1789,31 @@
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B3:J8"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B19:J19"/>
+    <mergeCell ref="C21:I29"/>
+    <mergeCell ref="E10:J10"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="B14:J14"/>
+    <mergeCell ref="E11:J12"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="G36:H38"/>
+    <mergeCell ref="I36:J38"/>
+    <mergeCell ref="B39:F41"/>
+    <mergeCell ref="G39:H41"/>
+    <mergeCell ref="I39:J41"/>
+    <mergeCell ref="G42:H44"/>
+    <mergeCell ref="I42:J44"/>
+    <mergeCell ref="B45:F47"/>
+    <mergeCell ref="G45:H47"/>
+    <mergeCell ref="I45:J47"/>
     <mergeCell ref="B49:C49"/>
     <mergeCell ref="D49:E49"/>
     <mergeCell ref="B48:C48"/>
@@ -1743,31 +1830,6 @@
     <mergeCell ref="I33:J35"/>
     <mergeCell ref="B17:J17"/>
     <mergeCell ref="B15:C15"/>
-    <mergeCell ref="G42:H44"/>
-    <mergeCell ref="I42:J44"/>
-    <mergeCell ref="B45:F47"/>
-    <mergeCell ref="G45:H47"/>
-    <mergeCell ref="I45:J47"/>
-    <mergeCell ref="G36:H38"/>
-    <mergeCell ref="I36:J38"/>
-    <mergeCell ref="B39:F41"/>
-    <mergeCell ref="G39:H41"/>
-    <mergeCell ref="I39:J41"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B3:J8"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B19:J19"/>
-    <mergeCell ref="C21:I29"/>
-    <mergeCell ref="E10:J10"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="B14:J14"/>
-    <mergeCell ref="E11:J12"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>